<commit_message>
update social+doors model 2
</commit_message>
<xml_diff>
--- a/derivatives/imaging_plots/istart_covariates_social+doors_2.xlsx
+++ b/derivatives/imaging_plots/istart_covariates_social+doors_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswyngaarden/Documents/Documents_Air/GitHub/istart-socdoors/derivatives/imaging_plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB08CFF-5D57-4A40-9D0E-55CAE69A1C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3303354D-6082-F54F-B700-F409483AC5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22740" yWindow="2700" windowWidth="14400" windowHeight="16520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model-2 social" sheetId="8" r:id="rId1"/>
@@ -502,7 +502,7 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>